<commit_message>
Update data kematian, PDRB, dan file dashboard
</commit_message>
<xml_diff>
--- a/Kependudukan Publikasi Softfile/Jumlah Kematian menurut Kelurahan dan Jenis Kelamin di Kota Mojokerto 2023.xlsx
+++ b/Kependudukan Publikasi Softfile/Jumlah Kematian menurut Kelurahan dan Jenis Kelamin di Kota Mojokerto 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\openpgsvc\Downloads\DARI PUBLIKASI SOFTFILE-20240825T224847Z-001\DARI PUBLIKASI SOFTFILE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F05C5B-0749-4D85-803A-F6B2A86BC2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7ACF93B-DC96-4BF4-AB2E-E7499643EF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D4079364-34CE-4E3C-AA6C-A6A5A798D112}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D4079364-34CE-4E3C-AA6C-A6A5A798D112}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,24 +172,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -509,7 +503,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,7 +544,7 @@
       <c r="D2" s="3">
         <v>2</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>5.71</v>
       </c>
     </row>
@@ -618,7 +612,7 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>2.86</v>
       </c>
     </row>
@@ -635,7 +629,7 @@
       <c r="D7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>2.86</v>
       </c>
     </row>
@@ -669,7 +663,7 @@
       <c r="D9" s="3">
         <v>33</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>94.29</v>
       </c>
     </row>
@@ -720,7 +714,7 @@
       <c r="D12" s="4">
         <v>28</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>80</v>
       </c>
     </row>
@@ -754,7 +748,7 @@
       <c r="D14" s="4">
         <v>1</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="4">
         <v>2.86</v>
       </c>
     </row>
@@ -771,7 +765,7 @@
       <c r="D15" s="4">
         <v>4</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <v>11.43</v>
       </c>
     </row>
@@ -907,7 +901,7 @@
       <c r="D23" s="3">
         <v>35</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="3">
         <v>100</v>
       </c>
     </row>

</xml_diff>